<commit_message>
alterações bd arc comp
</commit_message>
<xml_diff>
--- a/Arq. Comp/Analytics/analytics.xlsx
+++ b/Arq. Comp/Analytics/analytics.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="27">
   <si>
     <t>null</t>
   </si>
@@ -88,12 +88,30 @@
   <si>
     <t>Horas</t>
   </si>
+  <si>
+    <t>Ruim</t>
+  </si>
+  <si>
+    <t>Ideal</t>
+  </si>
+  <si>
+    <t>Alerta</t>
+  </si>
+  <si>
+    <t>Emergência</t>
+  </si>
+  <si>
+    <t>Critico</t>
+  </si>
+  <si>
+    <t>Luminosidade</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,8 +119,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,8 +184,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="28">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -523,11 +574,141 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -555,12 +736,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -581,29 +756,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -648,10 +802,79 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,6 +926,1873 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Luminosidade</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Analytics!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>segunda-feira</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Analytics!$C$8:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Analytics!$D$8:$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>979</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>912</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>789</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>476</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>604</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>562</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>637</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>757</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>781</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>839</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>935</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B789-4AB6-B0BA-B729A1DF7346}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Analytics!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>terça-feira</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Analytics!$C$8:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Analytics!$E$8:$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>967</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>842</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>804</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>684</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>655</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>528</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>521</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>636</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>823</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>905</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>967</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B789-4AB6-B0BA-B729A1DF7346}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Analytics!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>quarta-feira</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Analytics!$C$8:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Analytics!$F$8:$F$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>951</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>892</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>778</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>695</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>662</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>525</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>552</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>697</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>834</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>915</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>939</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B789-4AB6-B0BA-B729A1DF7346}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Analytics!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>quinta-feira</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Analytics!$C$8:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Analytics!$G$8:$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>953</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>902</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>793</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>665</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>561</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>665</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>796</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>856</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>978</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B789-4AB6-B0BA-B729A1DF7346}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Analytics!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sexta-feira</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Analytics!$C$8:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Analytics!$H$8:$H$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>927</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>862</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>810</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>686</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>615</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>614</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>705</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>799</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>863</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>935</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-B789-4AB6-B0BA-B729A1DF7346}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Analytics!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sábado</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Analytics!$C$8:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Analytics!$I$8:$I$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>952</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>903</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>790</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>753</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>637</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>551</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>558</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>611</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>715</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>772</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>917</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>938</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-B789-4AB6-B0BA-B729A1DF7346}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1261847952"/>
+        <c:axId val="1261840880"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1261847952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1261840880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1261840880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1028"/>
+          <c:min val="400"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Lux</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1261847952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -970,8 +3060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,96 +3081,96 @@
   <sheetData>
     <row r="1" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="3:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="55" t="s">
+      <c r="C2" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="D2" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="54" t="s">
+      <c r="E2" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="54" t="s">
+      <c r="F2" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="54" t="s">
+      <c r="G2" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="54" t="s">
+      <c r="H2" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="53" t="s">
+      <c r="I2" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="31"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="51" t="s">
+      <c r="J2" s="22"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="50" t="s">
+      <c r="M2" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="50" t="s">
+      <c r="N2" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="50" t="s">
+      <c r="O2" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="50" t="s">
+      <c r="P2" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="49" t="s">
+      <c r="Q2" s="40" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="3:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="48">
+      <c r="C3" s="39">
         <v>1</v>
       </c>
-      <c r="D3" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="45" t="s">
+      <c r="D3" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="43">
+      <c r="L3" s="34">
         <f ca="1">MIN(D8:D23)</f>
         <v>476</v>
       </c>
-      <c r="M3" s="42">
+      <c r="M3" s="33">
         <f ca="1">MIN(E8:E21)</f>
-        <v>518</v>
-      </c>
-      <c r="N3" s="42">
+        <v>521</v>
+      </c>
+      <c r="N3" s="33">
         <f ca="1">MIN(F8:F21)</f>
-        <v>570</v>
-      </c>
-      <c r="O3" s="42">
+        <v>525</v>
+      </c>
+      <c r="O3" s="33">
         <f ca="1">MIN(G8:G21)</f>
         <v>561</v>
       </c>
-      <c r="P3" s="42">
+      <c r="P3" s="33">
         <f ca="1">MIN(H8:H21)</f>
-        <v>568</v>
-      </c>
-      <c r="Q3" s="41">
+        <v>530</v>
+      </c>
+      <c r="Q3" s="32">
         <f ca="1">MIN(I8:I23)</f>
-        <v>578</v>
+        <v>551</v>
       </c>
     </row>
     <row r="4" spans="3:17" x14ac:dyDescent="0.25">
@@ -1105,32 +3195,32 @@
       <c r="I4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K4" s="44" t="s">
+      <c r="K4" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="43">
-        <f ca="1">_xlfn.QUARTILE.EXC(D8:D23,1)</f>
-        <v>626</v>
-      </c>
-      <c r="M4" s="42">
-        <f ca="1">_xlfn.QUARTILE.EXC(E8:E23,1)</f>
-        <v>659.75</v>
-      </c>
-      <c r="N4" s="42">
-        <f ca="1">_xlfn.QUARTILE.EXC(F8:F23,1)</f>
-        <v>669</v>
-      </c>
-      <c r="O4" s="42">
-        <f ca="1">_xlfn.QUARTILE.EXC(G8:G23,1)</f>
-        <v>674.5</v>
-      </c>
-      <c r="P4" s="42">
-        <f ca="1">_xlfn.QUARTILE.EXC(H8:H23,1)</f>
-        <v>654</v>
-      </c>
-      <c r="Q4" s="41">
-        <f ca="1">_xlfn.QUARTILE.EXC(I8:I23,1)</f>
-        <v>668.5</v>
+      <c r="L4" s="34">
+        <f t="shared" ref="L4:Q4" ca="1" si="0">_xlfn.QUARTILE.EXC(D8:D23,1)</f>
+        <v>612.25</v>
+      </c>
+      <c r="M4" s="33">
+        <f t="shared" ca="1" si="0"/>
+        <v>662.25</v>
+      </c>
+      <c r="N4" s="33">
+        <f t="shared" ca="1" si="0"/>
+        <v>670.25</v>
+      </c>
+      <c r="O4" s="33">
+        <f t="shared" ca="1" si="0"/>
+        <v>683.75</v>
+      </c>
+      <c r="P4" s="33">
+        <f t="shared" ca="1" si="0"/>
+        <v>632.75</v>
+      </c>
+      <c r="Q4" s="32">
+        <f t="shared" ca="1" si="0"/>
+        <v>656.5</v>
       </c>
     </row>
     <row r="5" spans="3:17" x14ac:dyDescent="0.25">
@@ -1155,32 +3245,32 @@
       <c r="I5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="44" t="s">
+      <c r="K5" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="43">
-        <f ca="1">MEDIAN(D8:D23)</f>
-        <v>853</v>
-      </c>
-      <c r="M5" s="42">
-        <f ca="1">MEDIAN(E8:E23)</f>
-        <v>804.5</v>
-      </c>
-      <c r="N5" s="42">
-        <f ca="1">MEDIAN(F8:F23)</f>
-        <v>840.5</v>
-      </c>
-      <c r="O5" s="42">
-        <f ca="1">MEDIAN(G8:G23)</f>
-        <v>827.5</v>
-      </c>
-      <c r="P5" s="42">
-        <f ca="1">MEDIAN(H8:H23)</f>
-        <v>849.5</v>
-      </c>
-      <c r="Q5" s="41">
-        <f ca="1">MEDIAN(I8:I23)</f>
-        <v>851</v>
+      <c r="L5" s="34">
+        <f t="shared" ref="L5:Q5" ca="1" si="1">MEDIAN(D8:D23)</f>
+        <v>814</v>
+      </c>
+      <c r="M5" s="33">
+        <f t="shared" ca="1" si="1"/>
+        <v>832.5</v>
+      </c>
+      <c r="N5" s="33">
+        <f t="shared" ca="1" si="1"/>
+        <v>863</v>
+      </c>
+      <c r="O5" s="33">
+        <f t="shared" ca="1" si="1"/>
+        <v>826</v>
+      </c>
+      <c r="P5" s="33">
+        <f t="shared" ca="1" si="1"/>
+        <v>836</v>
+      </c>
+      <c r="Q5" s="32">
+        <f t="shared" ca="1" si="1"/>
+        <v>846.5</v>
       </c>
     </row>
     <row r="6" spans="3:17" x14ac:dyDescent="0.25">
@@ -1205,32 +3295,32 @@
       <c r="I6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K6" s="44" t="s">
+      <c r="K6" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="43">
-        <f ca="1">_xlfn.QUARTILE.EXC(D8:D23,3)</f>
-        <v>998.75</v>
-      </c>
-      <c r="M6" s="42">
-        <f ca="1">_xlfn.QUARTILE.EXC(E8:E23,3)</f>
-        <v>995.75</v>
-      </c>
-      <c r="N6" s="42">
-        <f ca="1">_xlfn.QUARTILE.EXC(F8:F23,3)</f>
-        <v>996.5</v>
-      </c>
-      <c r="O6" s="42">
-        <f ca="1">_xlfn.QUARTILE.EXC(G8:G23,3)</f>
-        <v>999.25</v>
-      </c>
-      <c r="P6" s="42">
-        <f ca="1">_xlfn.QUARTILE.EXC(H8:H23,3)</f>
-        <v>996.75</v>
-      </c>
-      <c r="Q6" s="41">
-        <f ca="1">_xlfn.QUARTILE.EXC(I8:I23,3)</f>
-        <v>987.25</v>
+      <c r="L6" s="34">
+        <f t="shared" ref="L6:Q6" ca="1" si="2">_xlfn.QUARTILE.EXC(D8:D23,3)</f>
+        <v>994.75</v>
+      </c>
+      <c r="M6" s="33">
+        <f t="shared" ca="1" si="2"/>
+        <v>991.75</v>
+      </c>
+      <c r="N6" s="33">
+        <f t="shared" ca="1" si="2"/>
+        <v>987.75</v>
+      </c>
+      <c r="O6" s="33">
+        <f t="shared" ca="1" si="2"/>
+        <v>994.5</v>
+      </c>
+      <c r="P6" s="33">
+        <f t="shared" ca="1" si="2"/>
+        <v>983.75</v>
+      </c>
+      <c r="Q6" s="32">
+        <f t="shared" ca="1" si="2"/>
+        <v>988</v>
       </c>
     </row>
     <row r="7" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1255,31 +3345,31 @@
       <c r="I7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K7" s="40" t="s">
+      <c r="K7" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="39">
-        <f ca="1">MAX(D8:D23)</f>
+      <c r="L7" s="30">
+        <f t="shared" ref="L7:Q7" ca="1" si="3">MAX(D8:D23)</f>
         <v>1000</v>
       </c>
-      <c r="M7" s="38">
-        <f ca="1">MAX(E8:E23)</f>
+      <c r="M7" s="29">
+        <f t="shared" ca="1" si="3"/>
         <v>1000</v>
       </c>
-      <c r="N7" s="38">
-        <f ca="1">MAX(F8:F23)</f>
+      <c r="N7" s="29">
+        <f t="shared" ca="1" si="3"/>
         <v>1000</v>
       </c>
-      <c r="O7" s="38">
-        <f ca="1">MAX(G8:G23)</f>
+      <c r="O7" s="29">
+        <f t="shared" ca="1" si="3"/>
         <v>1000</v>
       </c>
-      <c r="P7" s="38">
-        <f ca="1">MAX(H8:H23)</f>
+      <c r="P7" s="29">
+        <f t="shared" ca="1" si="3"/>
         <v>1000</v>
       </c>
-      <c r="Q7" s="37">
-        <f ca="1">MAX(I8:I23)</f>
+      <c r="Q7" s="28">
+        <f t="shared" ca="1" si="3"/>
         <v>1000</v>
       </c>
     </row>
@@ -1302,38 +3392,38 @@
       <c r="H8" s="5">
         <v>1000</v>
       </c>
-      <c r="I8" s="36">
+      <c r="I8" s="27">
         <v>1000</v>
       </c>
-      <c r="J8" s="13"/>
+      <c r="J8" s="11"/>
     </row>
     <row r="9" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="4">
         <v>7</v>
       </c>
       <c r="D9" s="7">
-        <f ca="1">RANDBETWEEN(920,1000)</f>
-        <v>995</v>
+        <f t="shared" ref="D9:I9" ca="1" si="4">RANDBETWEEN(920,1000)</f>
+        <v>979</v>
       </c>
       <c r="E9" s="7">
-        <f ca="1">RANDBETWEEN(920,1000)</f>
-        <v>983</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>967</v>
       </c>
       <c r="F9" s="7">
-        <f ca="1">RANDBETWEEN(920,1000)</f>
-        <v>959</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>951</v>
       </c>
       <c r="G9" s="7">
-        <f ca="1">RANDBETWEEN(920,1000)</f>
-        <v>997</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>953</v>
       </c>
       <c r="H9" s="7">
-        <f ca="1">RANDBETWEEN(920,1000)</f>
-        <v>987</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>927</v>
       </c>
       <c r="I9" s="6">
-        <f ca="1">RANDBETWEEN(920,1000)</f>
-        <v>949</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>952</v>
       </c>
       <c r="K9" t="s">
         <v>8</v>
@@ -1344,55 +3434,55 @@
         <v>8</v>
       </c>
       <c r="D10" s="7">
-        <f ca="1">RANDBETWEEN(839,919)</f>
-        <v>891</v>
+        <f t="shared" ref="D10:I10" ca="1" si="5">RANDBETWEEN(839,919)</f>
+        <v>912</v>
       </c>
       <c r="E10" s="7">
-        <f ca="1">RANDBETWEEN(839,919)</f>
-        <v>885</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>842</v>
       </c>
       <c r="F10" s="7">
-        <f ca="1">RANDBETWEEN(839,919)</f>
-        <v>879</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>892</v>
       </c>
       <c r="G10" s="7">
-        <f ca="1">RANDBETWEEN(839,919)</f>
-        <v>848</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>902</v>
       </c>
       <c r="H10" s="7">
-        <f ca="1">RANDBETWEEN(839,919)</f>
-        <v>908</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>862</v>
       </c>
       <c r="I10" s="6">
-        <f ca="1">RANDBETWEEN(839,919)</f>
-        <v>884</v>
-      </c>
-      <c r="K10" s="35" t="s">
+        <f t="shared" ca="1" si="5"/>
+        <v>903</v>
+      </c>
+      <c r="K10" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="L10" s="34">
-        <f ca="1">AVERAGE(D8:D23)</f>
-        <v>805.8125</v>
-      </c>
-      <c r="M10" s="33">
-        <f ca="1">AVERAGE(E8:E23)</f>
-        <v>811.5625</v>
-      </c>
-      <c r="N10" s="33">
-        <f ca="1">AVERAGE(F8:F23)</f>
-        <v>823.875</v>
-      </c>
-      <c r="O10" s="33">
-        <f ca="1">AVERAGE(G8:G23)</f>
-        <v>820.9375</v>
-      </c>
-      <c r="P10" s="33">
-        <f ca="1">AVERAGE(H8:H23)</f>
-        <v>821.125</v>
-      </c>
-      <c r="Q10" s="32">
-        <f ca="1">AVERAGE(I8:I23)</f>
-        <v>821.875</v>
+      <c r="L10" s="25">
+        <f t="shared" ref="L10:Q10" ca="1" si="6">AVERAGE(D8:D23)</f>
+        <v>802.5625</v>
+      </c>
+      <c r="M10" s="24">
+        <f t="shared" ca="1" si="6"/>
+        <v>813.875</v>
+      </c>
+      <c r="N10" s="24">
+        <f t="shared" ca="1" si="6"/>
+        <v>815</v>
+      </c>
+      <c r="O10" s="24">
+        <f t="shared" ca="1" si="6"/>
+        <v>827.1875</v>
+      </c>
+      <c r="P10" s="24">
+        <f t="shared" ca="1" si="6"/>
+        <v>805.375</v>
+      </c>
+      <c r="Q10" s="23">
+        <f t="shared" ca="1" si="6"/>
+        <v>818.5625</v>
       </c>
     </row>
     <row r="11" spans="3:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1400,340 +3490,340 @@
         <v>9</v>
       </c>
       <c r="D11" s="9">
-        <f ca="1">RANDBETWEEN(759,838)</f>
-        <v>794</v>
+        <f t="shared" ref="D11:I11" ca="1" si="7">RANDBETWEEN(759,838)</f>
+        <v>789</v>
       </c>
       <c r="E11" s="9">
-        <f ca="1">RANDBETWEEN(759,838)</f>
-        <v>764</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>804</v>
       </c>
       <c r="F11" s="9">
-        <f ca="1">RANDBETWEEN(759,838)</f>
-        <v>762</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>778</v>
       </c>
       <c r="G11" s="9">
-        <f ca="1">RANDBETWEEN(759,838)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>793</v>
       </c>
       <c r="H11" s="9">
-        <f ca="1">RANDBETWEEN(759,838)</f>
-        <v>761</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>810</v>
       </c>
       <c r="I11" s="8">
-        <f ca="1">RANDBETWEEN(759,838)</f>
-        <v>818</v>
-      </c>
-      <c r="J11" s="31"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
+        <f t="shared" ca="1" si="7"/>
+        <v>790</v>
+      </c>
+      <c r="J11" s="22"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
     </row>
     <row r="12" spans="3:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="4">
         <v>10</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="21">
         <v>476</v>
       </c>
       <c r="E12" s="9">
         <f ca="1">RANDBETWEEN(677,757)</f>
-        <v>677</v>
-      </c>
-      <c r="F12" s="15">
+        <v>684</v>
+      </c>
+      <c r="F12" s="13">
         <f ca="1">RANDBETWEEN(677,757)</f>
-        <v>724</v>
-      </c>
-      <c r="G12" s="15">
+        <v>695</v>
+      </c>
+      <c r="G12" s="13">
         <f ca="1">RANDBETWEEN(677,757)</f>
-        <v>718</v>
-      </c>
-      <c r="H12" s="15">
+        <v>751</v>
+      </c>
+      <c r="H12" s="13">
         <f ca="1">RANDBETWEEN(677,757)</f>
-        <v>714</v>
-      </c>
-      <c r="I12" s="14">
+        <v>686</v>
+      </c>
+      <c r="I12" s="12">
         <f ca="1">RANDBETWEEN(677,757)</f>
-        <v>721</v>
-      </c>
-      <c r="K12" s="19"/>
-      <c r="L12" s="29" t="s">
+        <v>753</v>
+      </c>
+      <c r="K12" s="17"/>
+      <c r="L12" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="27"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="63"/>
+      <c r="O12" s="64"/>
     </row>
     <row r="13" spans="3:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C13" s="4">
         <v>11</v>
       </c>
-      <c r="D13" s="15">
-        <f ca="1">RANDBETWEEN(596,676)</f>
-        <v>611</v>
-      </c>
-      <c r="E13" s="15">
-        <f ca="1">RANDBETWEEN(596,676)</f>
-        <v>654</v>
-      </c>
-      <c r="F13" s="15">
-        <f ca="1">RANDBETWEEN(596,676)</f>
-        <v>630</v>
-      </c>
-      <c r="G13" s="15">
-        <f ca="1">RANDBETWEEN(596,676)</f>
+      <c r="D13" s="13">
+        <f t="shared" ref="D13:I13" ca="1" si="8">RANDBETWEEN(596,676)</f>
+        <v>604</v>
+      </c>
+      <c r="E13" s="13">
+        <f t="shared" ca="1" si="8"/>
+        <v>655</v>
+      </c>
+      <c r="F13" s="13">
+        <f t="shared" ca="1" si="8"/>
+        <v>662</v>
+      </c>
+      <c r="G13" s="13">
+        <f t="shared" ca="1" si="8"/>
+        <v>665</v>
+      </c>
+      <c r="H13" s="13">
+        <f t="shared" ca="1" si="8"/>
         <v>615</v>
       </c>
-      <c r="H13" s="15">
-        <f ca="1">RANDBETWEEN(596,676)</f>
-        <v>612</v>
-      </c>
-      <c r="I13" s="14">
-        <f ca="1">RANDBETWEEN(596,676)</f>
-        <v>615</v>
-      </c>
-      <c r="K13" s="19"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="25" t="s">
+      <c r="I13" s="12">
+        <f t="shared" ca="1" si="8"/>
+        <v>637</v>
+      </c>
+      <c r="K13" s="17"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="N13" s="25"/>
-      <c r="O13" s="24"/>
+      <c r="N13" s="65"/>
+      <c r="O13" s="66"/>
     </row>
     <row r="14" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C14" s="4">
         <v>12</v>
       </c>
-      <c r="D14" s="15">
-        <f ca="1">RANDBETWEEN(515,595)</f>
-        <v>539</v>
-      </c>
-      <c r="E14" s="15">
-        <f ca="1">RANDBETWEEN(515,595)</f>
-        <v>590</v>
-      </c>
-      <c r="F14" s="15">
-        <f ca="1">RANDBETWEEN(515,595)</f>
-        <v>588</v>
-      </c>
-      <c r="G14" s="15">
-        <f ca="1">RANDBETWEEN(515,595)</f>
-        <v>561</v>
-      </c>
-      <c r="H14" s="15">
-        <f ca="1">RANDBETWEEN(515,595)</f>
-        <v>583</v>
-      </c>
-      <c r="I14" s="14">
-        <f ca="1">RANDBETWEEN(515,595)</f>
-        <v>578</v>
-      </c>
-      <c r="K14" s="19"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="22" t="s">
+      <c r="D14" s="13">
+        <f t="shared" ref="D14:I15" ca="1" si="9">RANDBETWEEN(515,595)</f>
+        <v>562</v>
+      </c>
+      <c r="E14" s="13">
+        <f t="shared" ca="1" si="9"/>
+        <v>528</v>
+      </c>
+      <c r="F14" s="13">
+        <f t="shared" ca="1" si="9"/>
+        <v>525</v>
+      </c>
+      <c r="G14" s="13">
+        <f t="shared" ca="1" si="9"/>
+        <v>575</v>
+      </c>
+      <c r="H14" s="13">
+        <f t="shared" ca="1" si="9"/>
+        <v>530</v>
+      </c>
+      <c r="I14" s="12">
+        <f t="shared" ca="1" si="9"/>
+        <v>551</v>
+      </c>
+      <c r="K14" s="17"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="N14" s="22"/>
-      <c r="O14" s="21"/>
+      <c r="N14" s="60"/>
+      <c r="O14" s="61"/>
     </row>
     <row r="15" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C15" s="4">
         <v>13</v>
       </c>
-      <c r="D15" s="15">
-        <f ca="1">RANDBETWEEN(515,595)</f>
-        <v>532</v>
-      </c>
-      <c r="E15" s="15">
-        <f ca="1">RANDBETWEEN(515,595)</f>
-        <v>518</v>
-      </c>
-      <c r="F15" s="15">
-        <f ca="1">RANDBETWEEN(515,595)</f>
+      <c r="D15" s="13">
+        <f t="shared" ca="1" si="9"/>
         <v>570</v>
       </c>
-      <c r="G15" s="15">
-        <f ca="1">RANDBETWEEN(515,595)</f>
-        <v>567</v>
-      </c>
-      <c r="H15" s="15">
-        <f ca="1">RANDBETWEEN(515,595)</f>
-        <v>568</v>
-      </c>
-      <c r="I15" s="14">
-        <f ca="1">RANDBETWEEN(515,595)</f>
-        <v>591</v>
-      </c>
-      <c r="K15" s="19"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="11" t="s">
+      <c r="E15" s="13">
+        <f t="shared" ca="1" si="9"/>
+        <v>521</v>
+      </c>
+      <c r="F15" s="13">
+        <f t="shared" ca="1" si="9"/>
+        <v>552</v>
+      </c>
+      <c r="G15" s="13">
+        <f t="shared" ca="1" si="9"/>
+        <v>561</v>
+      </c>
+      <c r="H15" s="13">
+        <f t="shared" ca="1" si="9"/>
+        <v>540</v>
+      </c>
+      <c r="I15" s="12">
+        <f t="shared" ca="1" si="9"/>
+        <v>558</v>
+      </c>
+      <c r="K15" s="17"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="N15" s="11"/>
-      <c r="O15" s="10"/>
+      <c r="N15" s="58"/>
+      <c r="O15" s="59"/>
     </row>
     <row r="16" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C16" s="4">
         <v>14</v>
       </c>
-      <c r="D16" s="15">
-        <f ca="1">RANDBETWEEN(596,676)</f>
-        <v>671</v>
-      </c>
-      <c r="E16" s="15">
-        <f ca="1">RANDBETWEEN(596,676)</f>
-        <v>625</v>
-      </c>
-      <c r="F16" s="15">
-        <f ca="1">RANDBETWEEN(596,676)</f>
-        <v>656</v>
-      </c>
-      <c r="G16" s="15">
-        <f ca="1">RANDBETWEEN(596,676)</f>
-        <v>660</v>
-      </c>
-      <c r="H16" s="15">
-        <f ca="1">RANDBETWEEN(596,676)</f>
-        <v>644</v>
-      </c>
-      <c r="I16" s="14">
-        <f ca="1">RANDBETWEEN(596,676)</f>
-        <v>651</v>
-      </c>
-      <c r="K16" s="19"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="17" t="s">
+      <c r="D16" s="13">
+        <f t="shared" ref="D16:I16" ca="1" si="10">RANDBETWEEN(596,676)</f>
+        <v>637</v>
+      </c>
+      <c r="E16" s="13">
+        <f t="shared" ca="1" si="10"/>
+        <v>636</v>
+      </c>
+      <c r="F16" s="13">
+        <f t="shared" ca="1" si="10"/>
+        <v>600</v>
+      </c>
+      <c r="G16" s="13">
+        <f t="shared" ca="1" si="10"/>
+        <v>665</v>
+      </c>
+      <c r="H16" s="13">
+        <f t="shared" ca="1" si="10"/>
+        <v>614</v>
+      </c>
+      <c r="I16" s="12">
+        <f t="shared" ca="1" si="10"/>
+        <v>611</v>
+      </c>
+      <c r="K16" s="17"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="N16" s="17"/>
-      <c r="O16" s="16"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="14"/>
     </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C17" s="4">
         <v>15</v>
       </c>
-      <c r="D17" s="15">
-        <f ca="1">RANDBETWEEN(677,757)</f>
-        <v>736</v>
-      </c>
-      <c r="E17" s="15">
-        <f ca="1">RANDBETWEEN(677,757)</f>
-        <v>735</v>
-      </c>
-      <c r="F17" s="15">
-        <f ca="1">RANDBETWEEN(677,757)</f>
-        <v>708</v>
-      </c>
-      <c r="G17" s="15">
-        <f ca="1">RANDBETWEEN(677,757)</f>
-        <v>756</v>
-      </c>
-      <c r="H17" s="15">
-        <f ca="1">RANDBETWEEN(677,757)</f>
-        <v>684</v>
-      </c>
-      <c r="I17" s="14">
-        <f ca="1">RANDBETWEEN(677,757)</f>
-        <v>746</v>
-      </c>
-      <c r="J17" s="13"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="11" t="s">
+      <c r="D17" s="13">
+        <f t="shared" ref="D17:I17" ca="1" si="11">RANDBETWEEN(677,757)</f>
+        <v>757</v>
+      </c>
+      <c r="E17" s="13">
+        <f t="shared" ca="1" si="11"/>
+        <v>690</v>
+      </c>
+      <c r="F17" s="13">
+        <f t="shared" ca="1" si="11"/>
+        <v>697</v>
+      </c>
+      <c r="G17" s="13">
+        <f t="shared" ca="1" si="11"/>
+        <v>740</v>
+      </c>
+      <c r="H17" s="13">
+        <f t="shared" ca="1" si="11"/>
+        <v>705</v>
+      </c>
+      <c r="I17" s="12">
+        <f t="shared" ca="1" si="11"/>
+        <v>715</v>
+      </c>
+      <c r="J17" s="11"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="N17" s="11"/>
-      <c r="O17" s="10"/>
+      <c r="N17" s="58"/>
+      <c r="O17" s="59"/>
     </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C18" s="4">
         <v>16</v>
       </c>
       <c r="D18" s="9">
-        <f ca="1">RANDBETWEEN(759,838)</f>
-        <v>826</v>
+        <f t="shared" ref="D18:I18" ca="1" si="12">RANDBETWEEN(759,838)</f>
+        <v>781</v>
       </c>
       <c r="E18" s="9">
-        <f ca="1">RANDBETWEEN(759,838)</f>
-        <v>763</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>823</v>
       </c>
       <c r="F18" s="9">
-        <f ca="1">RANDBETWEEN(759,838)</f>
-        <v>802</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>834</v>
       </c>
       <c r="G18" s="9">
-        <f ca="1">RANDBETWEEN(759,838)</f>
-        <v>807</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>796</v>
       </c>
       <c r="H18" s="9">
-        <f ca="1">RANDBETWEEN(759,838)</f>
-        <v>791</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>799</v>
       </c>
       <c r="I18" s="8">
-        <f ca="1">RANDBETWEEN(759,838)</f>
-        <v>765</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>772</v>
       </c>
     </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C19" s="4">
         <v>17</v>
       </c>
       <c r="D19" s="7">
-        <f ca="1">RANDBETWEEN(839,919)</f>
-        <v>880</v>
+        <f t="shared" ref="D19:I19" ca="1" si="13">RANDBETWEEN(839,919)</f>
+        <v>839</v>
       </c>
       <c r="E19" s="7">
-        <f ca="1">RANDBETWEEN(839,919)</f>
-        <v>845</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>905</v>
       </c>
       <c r="F19" s="7">
-        <f ca="1">RANDBETWEEN(839,919)</f>
-        <v>918</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>915</v>
       </c>
       <c r="G19" s="7">
-        <f ca="1">RANDBETWEEN(839,919)</f>
-        <v>853</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>856</v>
       </c>
       <c r="H19" s="7">
-        <f ca="1">RANDBETWEEN(839,919)</f>
+        <f t="shared" ca="1" si="13"/>
+        <v>863</v>
+      </c>
+      <c r="I19" s="6">
+        <f t="shared" ca="1" si="13"/>
         <v>917</v>
       </c>
-      <c r="I19" s="6">
-        <f ca="1">RANDBETWEEN(839,919)</f>
-        <v>895</v>
-      </c>
     </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="4">
         <v>18</v>
       </c>
       <c r="D20" s="7">
-        <f ca="1">RANDBETWEEN(920,1000)</f>
-        <v>942</v>
+        <f t="shared" ref="D20:I20" ca="1" si="14">RANDBETWEEN(920,1000)</f>
+        <v>935</v>
       </c>
       <c r="E20" s="7">
-        <f ca="1">RANDBETWEEN(920,1000)</f>
-        <v>946</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>967</v>
       </c>
       <c r="F20" s="7">
-        <f ca="1">RANDBETWEEN(920,1000)</f>
-        <v>986</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>939</v>
       </c>
       <c r="G20" s="7">
-        <f ca="1">RANDBETWEEN(920,1000)</f>
-        <v>960</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>978</v>
       </c>
       <c r="H20" s="7">
-        <f ca="1">RANDBETWEEN(920,1000)</f>
-        <v>969</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>935</v>
       </c>
       <c r="I20" s="6">
-        <f ca="1">RANDBETWEEN(920,1000)</f>
-        <v>937</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>938</v>
       </c>
     </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C21" s="4">
         <v>19</v>
       </c>
@@ -1752,11 +3842,19 @@
       <c r="H21" s="5">
         <v>1000</v>
       </c>
-      <c r="I21" s="5">
+      <c r="I21" s="27">
         <v>1000</v>
       </c>
+      <c r="K21" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="L21" s="56"/>
+      <c r="M21" s="56"/>
+      <c r="N21" s="56"/>
+      <c r="O21" s="56"/>
+      <c r="P21" s="57"/>
     </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C22" s="4">
         <v>20</v>
       </c>
@@ -1775,11 +3873,27 @@
       <c r="H22" s="5">
         <v>1000</v>
       </c>
-      <c r="I22" s="5">
+      <c r="I22" s="27">
         <v>1000</v>
       </c>
+      <c r="K22" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="M22" s="54"/>
+      <c r="N22" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="O22" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="P22" s="49" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="4">
         <v>21</v>
       </c>
@@ -1798,11 +3912,29 @@
       <c r="H23" s="5">
         <v>1000</v>
       </c>
-      <c r="I23" s="5">
+      <c r="I23" s="27">
         <v>1000</v>
       </c>
+      <c r="K23" s="50">
+        <v>499</v>
+      </c>
+      <c r="L23" s="46">
+        <v>500</v>
+      </c>
+      <c r="M23" s="46">
+        <v>750</v>
+      </c>
+      <c r="N23" s="52">
+        <v>839</v>
+      </c>
+      <c r="O23" s="51">
+        <v>990</v>
+      </c>
+      <c r="P23" s="53">
+        <v>1000</v>
+      </c>
     </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C24" s="4">
         <v>22</v>
       </c>
@@ -1825,7 +3957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C25" s="4">
         <v>23</v>
       </c>
@@ -1848,32 +3980,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="3">
         <v>24</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I26" s="1" t="s">
+      <c r="D26" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="F26" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="I26" s="68" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="3:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="K21:P21"/>
     <mergeCell ref="M17:O17"/>
     <mergeCell ref="M14:O14"/>
     <mergeCell ref="L12:O12"/>
@@ -1903,5 +4037,6 @@
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>